<commit_message>
output stage with 1uf real caps
</commit_message>
<xml_diff>
--- a/audio/list.xlsx
+++ b/audio/list.xlsx
@@ -5,23 +5,25 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\software\HomeAutomation\doc\audio\rohm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\software\HomeAutomation\audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="parametricSearch" localSheetId="0">Sheet1!$E$1:$S$54</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="384">
   <si>
     <t>PartNumber</t>
   </si>
@@ -1179,6 +1181,36 @@
   </si>
   <si>
     <t>-39.77858</t>
+  </si>
+  <si>
+    <t>MKP1840</t>
+  </si>
+  <si>
+    <t>PHE426</t>
+  </si>
+  <si>
+    <t>R75</t>
+  </si>
+  <si>
+    <t>160VDC</t>
+  </si>
+  <si>
+    <t>250VDC</t>
+  </si>
+  <si>
+    <t>400VDC</t>
+  </si>
+  <si>
+    <t>630VDC</t>
+  </si>
+  <si>
+    <t>max V @ 40kHz</t>
+  </si>
+  <si>
+    <t>MKP4</t>
+  </si>
+  <si>
+    <t>MKP10</t>
   </si>
 </sst>
 </file>
@@ -4487,7 +4519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -5201,6 +5233,271 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2">
+        <v>0.47</v>
+      </c>
+      <c r="C2">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>33</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0.82</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f>21*SQRT(2.2)</f>
+        <v>31.148033645801785</v>
+      </c>
+      <c r="E11">
+        <f>E10/SQRT(B11/B10)</f>
+        <v>36.221540552549669</v>
+      </c>
+      <c r="F11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15">
+        <v>0.47</v>
+      </c>
+      <c r="E15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>0.68</v>
+      </c>
+      <c r="D17">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>29</v>
+      </c>
+      <c r="E19">
+        <f>E15/SQRT(B19/B15)</f>
+        <v>30.850445701804698</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>1.5</v>
+      </c>
+      <c r="D21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>382</v>
+      </c>
+      <c r="B23">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>13</v>
+      </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>383</v>
+      </c>
+      <c r="B28">
+        <v>0.47</v>
+      </c>
+      <c r="D28">
+        <v>23</v>
+      </c>
+      <c r="E28">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+      <c r="E30">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -5247,15 +5544,15 @@
         <v>0.88</v>
       </c>
       <c r="D2" s="8">
-        <f t="shared" ref="D2:D5" si="0">POWER(A2/SQRT(2)*C2,2)/B2</f>
+        <f>POWER(A2/SQRT(2)*C2,2)/B2</f>
         <v>65.436799999999991</v>
       </c>
       <c r="E2" s="8">
-        <f t="shared" ref="E2:E5" si="1">D2/C2</f>
+        <f>D2/C2</f>
         <v>74.359999999999985</v>
       </c>
       <c r="F2" s="8">
-        <f t="shared" ref="F2:F5" si="2">E2/A2</f>
+        <f>E2/A2</f>
         <v>2.8599999999999994</v>
       </c>
     </row>
@@ -5270,15 +5567,15 @@
         <v>0.88</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" si="0"/>
+        <f>POWER(A3/SQRT(2)*C3,2)/B3</f>
         <v>62.944200000000002</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" si="1"/>
+        <f>D3/C3</f>
         <v>71.527500000000003</v>
       </c>
       <c r="F3" s="8">
-        <f t="shared" si="2"/>
+        <f>E3/A3</f>
         <v>2.8050000000000002</v>
       </c>
     </row>
@@ -5293,15 +5590,15 @@
         <v>0.88</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" si="0"/>
+        <f>POWER(A4/SQRT(2)*C4,2)/B4</f>
         <v>60.499999999999986</v>
       </c>
       <c r="E4" s="8">
-        <f t="shared" si="1"/>
+        <f>D4/C4</f>
         <v>68.749999999999986</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" si="2"/>
+        <f>E4/A4</f>
         <v>2.7499999999999996</v>
       </c>
     </row>
@@ -5316,15 +5613,15 @@
         <v>0.88</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="0"/>
+        <f>POWER(A5/SQRT(2)*C5,2)/B5</f>
         <v>58.104199999999977</v>
       </c>
       <c r="E5" s="8">
-        <f t="shared" si="1"/>
+        <f>D5/C5</f>
         <v>66.027499999999975</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" si="2"/>
+        <f>E5/A5</f>
         <v>2.694999999999999</v>
       </c>
     </row>
@@ -5362,15 +5659,15 @@
         <v>0.88</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" ref="D7:D20" si="3">POWER(A7/SQRT(2)*C7,2)/B7</f>
+        <f t="shared" ref="D7:D20" si="0">POWER(A7/SQRT(2)*C7,2)/B7</f>
         <v>53.457799999999999</v>
       </c>
       <c r="E7" s="8">
-        <f t="shared" ref="E7:E20" si="4">D7/C7</f>
+        <f t="shared" ref="E7:E20" si="1">D7/C7</f>
         <v>60.747499999999995</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" ref="F7:F20" si="5">E7/A7</f>
+        <f t="shared" ref="F7:F20" si="2">E7/A7</f>
         <v>2.585</v>
       </c>
     </row>
@@ -5385,15 +5682,15 @@
         <v>0.88</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>51.207199999999993</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>58.189999999999991</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.5299999999999998</v>
       </c>
     </row>
@@ -5408,15 +5705,15 @@
         <v>0.88</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>49.004999999999995</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>55.687499999999993</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.4749999999999996</v>
       </c>
     </row>
@@ -5431,15 +5728,15 @@
         <v>0.88</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>46.851200000000006</v>
       </c>
       <c r="E10" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>53.240000000000009</v>
       </c>
       <c r="F10" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.4200000000000004</v>
       </c>
     </row>
@@ -5454,15 +5751,15 @@
         <v>0.88</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>44.745799999999988</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>50.847499999999989</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.3649999999999993</v>
       </c>
     </row>
@@ -5477,15 +5774,15 @@
         <v>0.88</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>42.688799999999993</v>
       </c>
       <c r="E12" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>48.509999999999991</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.3099999999999996</v>
       </c>
     </row>
@@ -5500,15 +5797,15 @@
         <v>0.88</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>40.680200000000006</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>46.227500000000006</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.2550000000000003</v>
       </c>
     </row>
@@ -5523,15 +5820,15 @@
         <v>0.88</v>
       </c>
       <c r="D14" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>38.719999999999992</v>
       </c>
       <c r="E14" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>43.999999999999993</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.1999999999999997</v>
       </c>
     </row>
@@ -5546,15 +5843,15 @@
         <v>0.88</v>
       </c>
       <c r="D15" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>36.808199999999999</v>
       </c>
       <c r="E15" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>41.827500000000001</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.145</v>
       </c>
     </row>
@@ -5569,15 +5866,15 @@
         <v>0.88</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>34.944799999999994</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>39.709999999999994</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.09</v>
       </c>
     </row>
@@ -5592,15 +5889,15 @@
         <v>0.88</v>
       </c>
       <c r="D17" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>81.795999999999978</v>
       </c>
       <c r="E17" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>92.949999999999974</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>3.5749999999999988</v>
       </c>
     </row>
@@ -5615,15 +5912,15 @@
         <v>0.88</v>
       </c>
       <c r="D18" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>78.680250000000001</v>
       </c>
       <c r="E18" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>89.409374999999997</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>3.5062500000000001</v>
       </c>
     </row>
@@ -5638,15 +5935,15 @@
         <v>0.88</v>
       </c>
       <c r="D19" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>75.624999999999972</v>
       </c>
       <c r="E19" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>85.937499999999972</v>
       </c>
       <c r="F19" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>3.4374999999999987</v>
       </c>
     </row>
@@ -5661,15 +5958,15 @@
         <v>0.88</v>
       </c>
       <c r="D20" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>72.630249999999961</v>
       </c>
       <c r="E20" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>82.534374999999955</v>
       </c>
       <c r="F20" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>3.3687499999999981</v>
       </c>
     </row>
@@ -5707,15 +6004,15 @@
         <v>0.88</v>
       </c>
       <c r="D22" s="8">
-        <f t="shared" ref="D22:D31" si="6">POWER(A22/SQRT(2)*C22,2)/B22</f>
+        <f t="shared" ref="D22:D31" si="3">POWER(A22/SQRT(2)*C22,2)/B22</f>
         <v>66.822249999999997</v>
       </c>
       <c r="E22" s="8">
-        <f t="shared" ref="E22:E31" si="7">D22/C22</f>
+        <f t="shared" ref="E22:E31" si="4">D22/C22</f>
         <v>75.934375000000003</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" ref="F22:F31" si="8">E22/A22</f>
+        <f t="shared" ref="F22:F31" si="5">E22/A22</f>
         <v>3.2312500000000002</v>
       </c>
     </row>
@@ -5730,15 +6027,15 @@
         <v>0.88</v>
       </c>
       <c r="D23" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>64.008999999999986</v>
       </c>
       <c r="E23" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>72.737499999999983</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3.1624999999999992</v>
       </c>
     </row>
@@ -5753,15 +6050,15 @@
         <v>0.88</v>
       </c>
       <c r="D24" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>61.256249999999994</v>
       </c>
       <c r="E24" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>69.609375</v>
       </c>
       <c r="F24" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3.09375</v>
       </c>
     </row>
@@ -5776,15 +6073,15 @@
         <v>0.88</v>
       </c>
       <c r="D25" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>58.564000000000007</v>
       </c>
       <c r="E25" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>66.550000000000011</v>
       </c>
       <c r="F25" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>3.0250000000000004</v>
       </c>
     </row>
@@ -5799,15 +6096,15 @@
         <v>0.88</v>
       </c>
       <c r="D26" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>55.932249999999982</v>
       </c>
       <c r="E26" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>63.559374999999982</v>
       </c>
       <c r="F26" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2.9562499999999989</v>
       </c>
     </row>
@@ -5822,15 +6119,15 @@
         <v>0.88</v>
       </c>
       <c r="D27" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>53.36099999999999</v>
       </c>
       <c r="E27" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>60.637499999999989</v>
       </c>
       <c r="F27" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2.8874999999999993</v>
       </c>
     </row>
@@ -5845,15 +6142,15 @@
         <v>0.88</v>
       </c>
       <c r="D28" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>50.850250000000003</v>
       </c>
       <c r="E28" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>57.784375000000004</v>
       </c>
       <c r="F28" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2.8187500000000001</v>
       </c>
     </row>
@@ -5868,15 +6165,15 @@
         <v>0.88</v>
       </c>
       <c r="D29" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>48.399999999999984</v>
       </c>
       <c r="E29" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>54.999999999999979</v>
       </c>
       <c r="F29" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2.7499999999999991</v>
       </c>
     </row>
@@ -5891,15 +6188,15 @@
         <v>0.88</v>
       </c>
       <c r="D30" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>46.010249999999999</v>
       </c>
       <c r="E30" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>52.284374999999997</v>
       </c>
       <c r="F30" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2.6812499999999999</v>
       </c>
     </row>
@@ -5914,15 +6211,15 @@
         <v>0.88</v>
       </c>
       <c r="D31" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>43.68099999999999</v>
       </c>
       <c r="E31" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>49.637499999999989</v>
       </c>
       <c r="F31" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>2.6124999999999994</v>
       </c>
     </row>
@@ -5932,7 +6229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
@@ -6552,7 +6849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>

</xml_diff>